<commit_message>
Fixed table 1 formatting
</commit_message>
<xml_diff>
--- a/data/allMetaboliteData.xlsx
+++ b/data/allMetaboliteData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388728BB-BDB7-40D6-9B69-FCB0A04A9A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E67E0A-1D40-4D7B-99EC-9DF1526EF06F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fresh" sheetId="1" r:id="rId1"/>
@@ -1723,11 +1723,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2319,35 +2319,35 @@
       <c r="AF3">
         <v>0</v>
       </c>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="4"/>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="4"/>
-      <c r="AO3" s="4"/>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="4"/>
-      <c r="AR3" s="4"/>
-      <c r="AS3" s="4"/>
-      <c r="AT3" s="4"/>
-      <c r="AU3" s="4"/>
-      <c r="AV3" s="4"/>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="4"/>
-      <c r="AY3" s="4"/>
-      <c r="AZ3" s="4"/>
-      <c r="BA3" s="4"/>
-      <c r="BB3" s="4"/>
-      <c r="BC3" s="4"/>
-      <c r="BD3" s="4"/>
-      <c r="BE3" s="4"/>
-      <c r="BF3" s="4"/>
-      <c r="BG3" s="4"/>
-      <c r="BH3" s="4"/>
-      <c r="BI3" s="4"/>
-      <c r="BJ3" s="4"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="3"/>
+      <c r="AV3" s="3"/>
+      <c r="AW3" s="3"/>
+      <c r="AX3" s="3"/>
+      <c r="AY3" s="3"/>
+      <c r="AZ3" s="3"/>
+      <c r="BA3" s="3"/>
+      <c r="BB3" s="3"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3"/>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
+      <c r="BI3" s="3"/>
+      <c r="BJ3" s="3"/>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2446,35 +2446,35 @@
       <c r="AF4">
         <v>0</v>
       </c>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="4"/>
-      <c r="AW4" s="4"/>
-      <c r="AX4" s="4"/>
-      <c r="AY4" s="4"/>
-      <c r="AZ4" s="4"/>
-      <c r="BA4" s="4"/>
-      <c r="BB4" s="4"/>
-      <c r="BC4" s="4"/>
-      <c r="BD4" s="4"/>
-      <c r="BE4" s="4"/>
-      <c r="BF4" s="4"/>
-      <c r="BG4" s="4"/>
-      <c r="BH4" s="4"/>
-      <c r="BI4" s="4"/>
-      <c r="BJ4" s="4"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="3"/>
+      <c r="AW4" s="3"/>
+      <c r="AX4" s="3"/>
+      <c r="AY4" s="3"/>
+      <c r="AZ4" s="3"/>
+      <c r="BA4" s="3"/>
+      <c r="BB4" s="3"/>
+      <c r="BC4" s="3"/>
+      <c r="BD4" s="3"/>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3"/>
+      <c r="BG4" s="3"/>
+      <c r="BH4" s="3"/>
+      <c r="BI4" s="3"/>
+      <c r="BJ4" s="3"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2573,35 +2573,35 @@
       <c r="AF5">
         <v>0</v>
       </c>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="4"/>
-      <c r="AL5" s="4"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
-      <c r="AP5" s="4"/>
-      <c r="AQ5" s="4"/>
-      <c r="AR5" s="4"/>
-      <c r="AS5" s="4"/>
-      <c r="AT5" s="4"/>
-      <c r="AU5" s="4"/>
-      <c r="AV5" s="4"/>
-      <c r="AW5" s="4"/>
-      <c r="AX5" s="4"/>
-      <c r="AY5" s="4"/>
-      <c r="AZ5" s="4"/>
-      <c r="BA5" s="4"/>
-      <c r="BB5" s="4"/>
-      <c r="BC5" s="4"/>
-      <c r="BD5" s="4"/>
-      <c r="BE5" s="4"/>
-      <c r="BF5" s="4"/>
-      <c r="BG5" s="4"/>
-      <c r="BH5" s="4"/>
-      <c r="BI5" s="4"/>
-      <c r="BJ5" s="4"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AT5" s="3"/>
+      <c r="AU5" s="3"/>
+      <c r="AV5" s="3"/>
+      <c r="AW5" s="3"/>
+      <c r="AX5" s="3"/>
+      <c r="AY5" s="3"/>
+      <c r="AZ5" s="3"/>
+      <c r="BA5" s="3"/>
+      <c r="BB5" s="3"/>
+      <c r="BC5" s="3"/>
+      <c r="BD5" s="3"/>
+      <c r="BE5" s="3"/>
+      <c r="BF5" s="3"/>
+      <c r="BG5" s="3"/>
+      <c r="BH5" s="3"/>
+      <c r="BI5" s="3"/>
+      <c r="BJ5" s="3"/>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2700,35 +2700,35 @@
       <c r="AF6">
         <v>1.38366379538905</v>
       </c>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="4"/>
-      <c r="AP6" s="4"/>
-      <c r="AQ6" s="4"/>
-      <c r="AR6" s="4"/>
-      <c r="AS6" s="4"/>
-      <c r="AT6" s="4"/>
-      <c r="AU6" s="4"/>
-      <c r="AV6" s="4"/>
-      <c r="AW6" s="4"/>
-      <c r="AX6" s="4"/>
-      <c r="AY6" s="4"/>
-      <c r="AZ6" s="4"/>
-      <c r="BA6" s="4"/>
-      <c r="BB6" s="4"/>
-      <c r="BC6" s="4"/>
-      <c r="BD6" s="4"/>
-      <c r="BE6" s="4"/>
-      <c r="BF6" s="4"/>
-      <c r="BG6" s="4"/>
-      <c r="BH6" s="4"/>
-      <c r="BI6" s="4"/>
-      <c r="BJ6" s="4"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
+      <c r="AV6" s="3"/>
+      <c r="AW6" s="3"/>
+      <c r="AX6" s="3"/>
+      <c r="AY6" s="3"/>
+      <c r="AZ6" s="3"/>
+      <c r="BA6" s="3"/>
+      <c r="BB6" s="3"/>
+      <c r="BC6" s="3"/>
+      <c r="BD6" s="3"/>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3"/>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="3"/>
+      <c r="BI6" s="3"/>
+      <c r="BJ6" s="3"/>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2827,35 +2827,35 @@
       <c r="AF7">
         <v>0.49761108741594601</v>
       </c>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="4"/>
-      <c r="AJ7" s="4"/>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="4"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="4"/>
-      <c r="AO7" s="4"/>
-      <c r="AP7" s="4"/>
-      <c r="AQ7" s="4"/>
-      <c r="AR7" s="4"/>
-      <c r="AS7" s="4"/>
-      <c r="AT7" s="4"/>
-      <c r="AU7" s="4"/>
-      <c r="AV7" s="4"/>
-      <c r="AW7" s="4"/>
-      <c r="AX7" s="4"/>
-      <c r="AY7" s="4"/>
-      <c r="AZ7" s="4"/>
-      <c r="BA7" s="4"/>
-      <c r="BB7" s="4"/>
-      <c r="BC7" s="4"/>
-      <c r="BD7" s="4"/>
-      <c r="BE7" s="4"/>
-      <c r="BF7" s="4"/>
-      <c r="BG7" s="4"/>
-      <c r="BH7" s="4"/>
-      <c r="BI7" s="4"/>
-      <c r="BJ7" s="4"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="3"/>
+      <c r="AW7" s="3"/>
+      <c r="AX7" s="3"/>
+      <c r="AY7" s="3"/>
+      <c r="AZ7" s="3"/>
+      <c r="BA7" s="3"/>
+      <c r="BB7" s="3"/>
+      <c r="BC7" s="3"/>
+      <c r="BD7" s="3"/>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
+      <c r="BI7" s="3"/>
+      <c r="BJ7" s="3"/>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2954,35 +2954,35 @@
       <c r="AF8">
         <v>0.67344853602305499</v>
       </c>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="4"/>
-      <c r="AJ8" s="4"/>
-      <c r="AK8" s="4"/>
-      <c r="AL8" s="4"/>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="4"/>
-      <c r="AO8" s="4"/>
-      <c r="AP8" s="4"/>
-      <c r="AQ8" s="4"/>
-      <c r="AR8" s="4"/>
-      <c r="AS8" s="4"/>
-      <c r="AT8" s="4"/>
-      <c r="AU8" s="4"/>
-      <c r="AV8" s="4"/>
-      <c r="AW8" s="4"/>
-      <c r="AX8" s="4"/>
-      <c r="AY8" s="4"/>
-      <c r="AZ8" s="4"/>
-      <c r="BA8" s="4"/>
-      <c r="BB8" s="4"/>
-      <c r="BC8" s="4"/>
-      <c r="BD8" s="4"/>
-      <c r="BE8" s="4"/>
-      <c r="BF8" s="4"/>
-      <c r="BG8" s="4"/>
-      <c r="BH8" s="4"/>
-      <c r="BI8" s="4"/>
-      <c r="BJ8" s="4"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+      <c r="AU8" s="3"/>
+      <c r="AV8" s="3"/>
+      <c r="AW8" s="3"/>
+      <c r="AX8" s="3"/>
+      <c r="AY8" s="3"/>
+      <c r="AZ8" s="3"/>
+      <c r="BA8" s="3"/>
+      <c r="BB8" s="3"/>
+      <c r="BC8" s="3"/>
+      <c r="BD8" s="3"/>
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3"/>
+      <c r="BG8" s="3"/>
+      <c r="BH8" s="3"/>
+      <c r="BI8" s="3"/>
+      <c r="BJ8" s="3"/>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3081,35 +3081,35 @@
       <c r="AF9">
         <v>0</v>
       </c>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="4"/>
-      <c r="AJ9" s="4"/>
-      <c r="AK9" s="4"/>
-      <c r="AL9" s="4"/>
-      <c r="AM9" s="4"/>
-      <c r="AN9" s="4"/>
-      <c r="AO9" s="4"/>
-      <c r="AP9" s="4"/>
-      <c r="AQ9" s="4"/>
-      <c r="AR9" s="4"/>
-      <c r="AS9" s="4"/>
-      <c r="AT9" s="4"/>
-      <c r="AU9" s="4"/>
-      <c r="AV9" s="4"/>
-      <c r="AW9" s="4"/>
-      <c r="AX9" s="4"/>
-      <c r="AY9" s="4"/>
-      <c r="AZ9" s="4"/>
-      <c r="BA9" s="4"/>
-      <c r="BB9" s="4"/>
-      <c r="BC9" s="4"/>
-      <c r="BD9" s="4"/>
-      <c r="BE9" s="4"/>
-      <c r="BF9" s="4"/>
-      <c r="BG9" s="4"/>
-      <c r="BH9" s="4"/>
-      <c r="BI9" s="4"/>
-      <c r="BJ9" s="4"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+      <c r="AU9" s="3"/>
+      <c r="AV9" s="3"/>
+      <c r="AW9" s="3"/>
+      <c r="AX9" s="3"/>
+      <c r="AY9" s="3"/>
+      <c r="AZ9" s="3"/>
+      <c r="BA9" s="3"/>
+      <c r="BB9" s="3"/>
+      <c r="BC9" s="3"/>
+      <c r="BD9" s="3"/>
+      <c r="BE9" s="3"/>
+      <c r="BF9" s="3"/>
+      <c r="BG9" s="3"/>
+      <c r="BH9" s="3"/>
+      <c r="BI9" s="3"/>
+      <c r="BJ9" s="3"/>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3208,35 +3208,35 @@
       <c r="AF10">
         <v>0</v>
       </c>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="4"/>
-      <c r="AJ10" s="4"/>
-      <c r="AK10" s="4"/>
-      <c r="AL10" s="4"/>
-      <c r="AM10" s="4"/>
-      <c r="AN10" s="4"/>
-      <c r="AO10" s="4"/>
-      <c r="AP10" s="4"/>
-      <c r="AQ10" s="4"/>
-      <c r="AR10" s="4"/>
-      <c r="AS10" s="4"/>
-      <c r="AT10" s="4"/>
-      <c r="AU10" s="4"/>
-      <c r="AV10" s="4"/>
-      <c r="AW10" s="4"/>
-      <c r="AX10" s="4"/>
-      <c r="AY10" s="4"/>
-      <c r="AZ10" s="4"/>
-      <c r="BA10" s="4"/>
-      <c r="BB10" s="4"/>
-      <c r="BC10" s="4"/>
-      <c r="BD10" s="4"/>
-      <c r="BE10" s="4"/>
-      <c r="BF10" s="4"/>
-      <c r="BG10" s="4"/>
-      <c r="BH10" s="4"/>
-      <c r="BI10" s="4"/>
-      <c r="BJ10" s="4"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+      <c r="AU10" s="3"/>
+      <c r="AV10" s="3"/>
+      <c r="AW10" s="3"/>
+      <c r="AX10" s="3"/>
+      <c r="AY10" s="3"/>
+      <c r="AZ10" s="3"/>
+      <c r="BA10" s="3"/>
+      <c r="BB10" s="3"/>
+      <c r="BC10" s="3"/>
+      <c r="BD10" s="3"/>
+      <c r="BE10" s="3"/>
+      <c r="BF10" s="3"/>
+      <c r="BG10" s="3"/>
+      <c r="BH10" s="3"/>
+      <c r="BI10" s="3"/>
+      <c r="BJ10" s="3"/>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3335,35 +3335,35 @@
       <c r="AF11">
         <v>9.4251911623438999E-3</v>
       </c>
-      <c r="AH11" s="4"/>
-      <c r="AI11" s="4"/>
-      <c r="AJ11" s="4"/>
-      <c r="AK11" s="4"/>
-      <c r="AL11" s="4"/>
-      <c r="AM11" s="4"/>
-      <c r="AN11" s="4"/>
-      <c r="AO11" s="4"/>
-      <c r="AP11" s="4"/>
-      <c r="AQ11" s="4"/>
-      <c r="AR11" s="4"/>
-      <c r="AS11" s="4"/>
-      <c r="AT11" s="4"/>
-      <c r="AU11" s="4"/>
-      <c r="AV11" s="4"/>
-      <c r="AW11" s="4"/>
-      <c r="AX11" s="4"/>
-      <c r="AY11" s="4"/>
-      <c r="AZ11" s="4"/>
-      <c r="BA11" s="4"/>
-      <c r="BB11" s="4"/>
-      <c r="BC11" s="4"/>
-      <c r="BD11" s="4"/>
-      <c r="BE11" s="4"/>
-      <c r="BF11" s="4"/>
-      <c r="BG11" s="4"/>
-      <c r="BH11" s="4"/>
-      <c r="BI11" s="4"/>
-      <c r="BJ11" s="4"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+      <c r="AU11" s="3"/>
+      <c r="AV11" s="3"/>
+      <c r="AW11" s="3"/>
+      <c r="AX11" s="3"/>
+      <c r="AY11" s="3"/>
+      <c r="AZ11" s="3"/>
+      <c r="BA11" s="3"/>
+      <c r="BB11" s="3"/>
+      <c r="BC11" s="3"/>
+      <c r="BD11" s="3"/>
+      <c r="BE11" s="3"/>
+      <c r="BF11" s="3"/>
+      <c r="BG11" s="3"/>
+      <c r="BH11" s="3"/>
+      <c r="BI11" s="3"/>
+      <c r="BJ11" s="3"/>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3462,35 +3462,35 @@
       <c r="AF12">
         <v>0</v>
       </c>
-      <c r="AH12" s="4"/>
-      <c r="AI12" s="4"/>
-      <c r="AJ12" s="4"/>
-      <c r="AK12" s="4"/>
-      <c r="AL12" s="4"/>
-      <c r="AM12" s="4"/>
-      <c r="AN12" s="4"/>
-      <c r="AO12" s="4"/>
-      <c r="AP12" s="4"/>
-      <c r="AQ12" s="4"/>
-      <c r="AR12" s="4"/>
-      <c r="AS12" s="4"/>
-      <c r="AT12" s="4"/>
-      <c r="AU12" s="4"/>
-      <c r="AV12" s="4"/>
-      <c r="AW12" s="4"/>
-      <c r="AX12" s="4"/>
-      <c r="AY12" s="4"/>
-      <c r="AZ12" s="4"/>
-      <c r="BA12" s="4"/>
-      <c r="BB12" s="4"/>
-      <c r="BC12" s="4"/>
-      <c r="BD12" s="4"/>
-      <c r="BE12" s="4"/>
-      <c r="BF12" s="4"/>
-      <c r="BG12" s="4"/>
-      <c r="BH12" s="4"/>
-      <c r="BI12" s="4"/>
-      <c r="BJ12" s="4"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+      <c r="AU12" s="3"/>
+      <c r="AV12" s="3"/>
+      <c r="AW12" s="3"/>
+      <c r="AX12" s="3"/>
+      <c r="AY12" s="3"/>
+      <c r="AZ12" s="3"/>
+      <c r="BA12" s="3"/>
+      <c r="BB12" s="3"/>
+      <c r="BC12" s="3"/>
+      <c r="BD12" s="3"/>
+      <c r="BE12" s="3"/>
+      <c r="BF12" s="3"/>
+      <c r="BG12" s="3"/>
+      <c r="BH12" s="3"/>
+      <c r="BI12" s="3"/>
+      <c r="BJ12" s="3"/>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3589,35 +3589,35 @@
       <c r="AF13">
         <v>0.27211564553314099</v>
       </c>
-      <c r="AH13" s="4"/>
-      <c r="AI13" s="4"/>
-      <c r="AJ13" s="4"/>
-      <c r="AK13" s="4"/>
-      <c r="AL13" s="4"/>
-      <c r="AM13" s="4"/>
-      <c r="AN13" s="4"/>
-      <c r="AO13" s="4"/>
-      <c r="AP13" s="4"/>
-      <c r="AQ13" s="4"/>
-      <c r="AR13" s="4"/>
-      <c r="AS13" s="4"/>
-      <c r="AT13" s="4"/>
-      <c r="AU13" s="4"/>
-      <c r="AV13" s="4"/>
-      <c r="AW13" s="4"/>
-      <c r="AX13" s="4"/>
-      <c r="AY13" s="4"/>
-      <c r="AZ13" s="4"/>
-      <c r="BA13" s="4"/>
-      <c r="BB13" s="4"/>
-      <c r="BC13" s="4"/>
-      <c r="BD13" s="4"/>
-      <c r="BE13" s="4"/>
-      <c r="BF13" s="4"/>
-      <c r="BG13" s="4"/>
-      <c r="BH13" s="4"/>
-      <c r="BI13" s="4"/>
-      <c r="BJ13" s="4"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="3"/>
+      <c r="AO13" s="3"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
+      <c r="AT13" s="3"/>
+      <c r="AU13" s="3"/>
+      <c r="AV13" s="3"/>
+      <c r="AW13" s="3"/>
+      <c r="AX13" s="3"/>
+      <c r="AY13" s="3"/>
+      <c r="AZ13" s="3"/>
+      <c r="BA13" s="3"/>
+      <c r="BB13" s="3"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3"/>
+      <c r="BG13" s="3"/>
+      <c r="BH13" s="3"/>
+      <c r="BI13" s="3"/>
+      <c r="BJ13" s="3"/>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3716,35 +3716,35 @@
       <c r="AF14">
         <v>0</v>
       </c>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="4"/>
-      <c r="AJ14" s="4"/>
-      <c r="AK14" s="4"/>
-      <c r="AL14" s="4"/>
-      <c r="AM14" s="4"/>
-      <c r="AN14" s="4"/>
-      <c r="AO14" s="4"/>
-      <c r="AP14" s="4"/>
-      <c r="AQ14" s="4"/>
-      <c r="AR14" s="4"/>
-      <c r="AS14" s="4"/>
-      <c r="AT14" s="4"/>
-      <c r="AU14" s="4"/>
-      <c r="AV14" s="4"/>
-      <c r="AW14" s="4"/>
-      <c r="AX14" s="4"/>
-      <c r="AY14" s="4"/>
-      <c r="AZ14" s="4"/>
-      <c r="BA14" s="4"/>
-      <c r="BB14" s="4"/>
-      <c r="BC14" s="4"/>
-      <c r="BD14" s="4"/>
-      <c r="BE14" s="4"/>
-      <c r="BF14" s="4"/>
-      <c r="BG14" s="4"/>
-      <c r="BH14" s="4"/>
-      <c r="BI14" s="4"/>
-      <c r="BJ14" s="4"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="3"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
+      <c r="AT14" s="3"/>
+      <c r="AU14" s="3"/>
+      <c r="AV14" s="3"/>
+      <c r="AW14" s="3"/>
+      <c r="AX14" s="3"/>
+      <c r="AY14" s="3"/>
+      <c r="AZ14" s="3"/>
+      <c r="BA14" s="3"/>
+      <c r="BB14" s="3"/>
+      <c r="BC14" s="3"/>
+      <c r="BD14" s="3"/>
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
+      <c r="BI14" s="3"/>
+      <c r="BJ14" s="3"/>
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3843,35 +3843,35 @@
       <c r="AF15">
         <v>0</v>
       </c>
-      <c r="AH15" s="4"/>
-      <c r="AI15" s="4"/>
-      <c r="AJ15" s="4"/>
-      <c r="AK15" s="4"/>
-      <c r="AL15" s="4"/>
-      <c r="AM15" s="4"/>
-      <c r="AN15" s="4"/>
-      <c r="AO15" s="4"/>
-      <c r="AP15" s="4"/>
-      <c r="AQ15" s="4"/>
-      <c r="AR15" s="4"/>
-      <c r="AS15" s="4"/>
-      <c r="AT15" s="4"/>
-      <c r="AU15" s="4"/>
-      <c r="AV15" s="4"/>
-      <c r="AW15" s="4"/>
-      <c r="AX15" s="4"/>
-      <c r="AY15" s="4"/>
-      <c r="AZ15" s="4"/>
-      <c r="BA15" s="4"/>
-      <c r="BB15" s="4"/>
-      <c r="BC15" s="4"/>
-      <c r="BD15" s="4"/>
-      <c r="BE15" s="4"/>
-      <c r="BF15" s="4"/>
-      <c r="BG15" s="4"/>
-      <c r="BH15" s="4"/>
-      <c r="BI15" s="4"/>
-      <c r="BJ15" s="4"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="3"/>
+      <c r="AN15" s="3"/>
+      <c r="AO15" s="3"/>
+      <c r="AP15" s="3"/>
+      <c r="AQ15" s="3"/>
+      <c r="AR15" s="3"/>
+      <c r="AS15" s="3"/>
+      <c r="AT15" s="3"/>
+      <c r="AU15" s="3"/>
+      <c r="AV15" s="3"/>
+      <c r="AW15" s="3"/>
+      <c r="AX15" s="3"/>
+      <c r="AY15" s="3"/>
+      <c r="AZ15" s="3"/>
+      <c r="BA15" s="3"/>
+      <c r="BB15" s="3"/>
+      <c r="BC15" s="3"/>
+      <c r="BD15" s="3"/>
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3"/>
+      <c r="BG15" s="3"/>
+      <c r="BH15" s="3"/>
+      <c r="BI15" s="3"/>
+      <c r="BJ15" s="3"/>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -3970,35 +3970,35 @@
       <c r="AF16">
         <v>0.26797114121037502</v>
       </c>
-      <c r="AH16" s="4"/>
-      <c r="AI16" s="4"/>
-      <c r="AJ16" s="4"/>
-      <c r="AK16" s="4"/>
-      <c r="AL16" s="4"/>
-      <c r="AM16" s="4"/>
-      <c r="AN16" s="4"/>
-      <c r="AO16" s="4"/>
-      <c r="AP16" s="4"/>
-      <c r="AQ16" s="4"/>
-      <c r="AR16" s="4"/>
-      <c r="AS16" s="4"/>
-      <c r="AT16" s="4"/>
-      <c r="AU16" s="4"/>
-      <c r="AV16" s="4"/>
-      <c r="AW16" s="4"/>
-      <c r="AX16" s="4"/>
-      <c r="AY16" s="4"/>
-      <c r="AZ16" s="4"/>
-      <c r="BA16" s="4"/>
-      <c r="BB16" s="4"/>
-      <c r="BC16" s="4"/>
-      <c r="BD16" s="4"/>
-      <c r="BE16" s="4"/>
-      <c r="BF16" s="4"/>
-      <c r="BG16" s="4"/>
-      <c r="BH16" s="4"/>
-      <c r="BI16" s="4"/>
-      <c r="BJ16" s="4"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="3"/>
+      <c r="AN16" s="3"/>
+      <c r="AO16" s="3"/>
+      <c r="AP16" s="3"/>
+      <c r="AQ16" s="3"/>
+      <c r="AR16" s="3"/>
+      <c r="AS16" s="3"/>
+      <c r="AT16" s="3"/>
+      <c r="AU16" s="3"/>
+      <c r="AV16" s="3"/>
+      <c r="AW16" s="3"/>
+      <c r="AX16" s="3"/>
+      <c r="AY16" s="3"/>
+      <c r="AZ16" s="3"/>
+      <c r="BA16" s="3"/>
+      <c r="BB16" s="3"/>
+      <c r="BC16" s="3"/>
+      <c r="BD16" s="3"/>
+      <c r="BE16" s="3"/>
+      <c r="BF16" s="3"/>
+      <c r="BG16" s="3"/>
+      <c r="BH16" s="3"/>
+      <c r="BI16" s="3"/>
+      <c r="BJ16" s="3"/>
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -4097,35 +4097,35 @@
       <c r="AF17">
         <v>0</v>
       </c>
-      <c r="AH17" s="4"/>
-      <c r="AI17" s="4"/>
-      <c r="AJ17" s="4"/>
-      <c r="AK17" s="4"/>
-      <c r="AL17" s="4"/>
-      <c r="AM17" s="4"/>
-      <c r="AN17" s="4"/>
-      <c r="AO17" s="4"/>
-      <c r="AP17" s="4"/>
-      <c r="AQ17" s="4"/>
-      <c r="AR17" s="4"/>
-      <c r="AS17" s="4"/>
-      <c r="AT17" s="4"/>
-      <c r="AU17" s="4"/>
-      <c r="AV17" s="4"/>
-      <c r="AW17" s="4"/>
-      <c r="AX17" s="4"/>
-      <c r="AY17" s="4"/>
-      <c r="AZ17" s="4"/>
-      <c r="BA17" s="4"/>
-      <c r="BB17" s="4"/>
-      <c r="BC17" s="4"/>
-      <c r="BD17" s="4"/>
-      <c r="BE17" s="4"/>
-      <c r="BF17" s="4"/>
-      <c r="BG17" s="4"/>
-      <c r="BH17" s="4"/>
-      <c r="BI17" s="4"/>
-      <c r="BJ17" s="4"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="3"/>
+      <c r="AN17" s="3"/>
+      <c r="AO17" s="3"/>
+      <c r="AP17" s="3"/>
+      <c r="AQ17" s="3"/>
+      <c r="AR17" s="3"/>
+      <c r="AS17" s="3"/>
+      <c r="AT17" s="3"/>
+      <c r="AU17" s="3"/>
+      <c r="AV17" s="3"/>
+      <c r="AW17" s="3"/>
+      <c r="AX17" s="3"/>
+      <c r="AY17" s="3"/>
+      <c r="AZ17" s="3"/>
+      <c r="BA17" s="3"/>
+      <c r="BB17" s="3"/>
+      <c r="BC17" s="3"/>
+      <c r="BD17" s="3"/>
+      <c r="BE17" s="3"/>
+      <c r="BF17" s="3"/>
+      <c r="BG17" s="3"/>
+      <c r="BH17" s="3"/>
+      <c r="BI17" s="3"/>
+      <c r="BJ17" s="3"/>
     </row>
     <row r="18" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -4224,35 +4224,35 @@
       <c r="AF18">
         <v>9.4481829747038102</v>
       </c>
-      <c r="AH18" s="4"/>
-      <c r="AI18" s="4"/>
-      <c r="AJ18" s="4"/>
-      <c r="AK18" s="4"/>
-      <c r="AL18" s="4"/>
-      <c r="AM18" s="4"/>
-      <c r="AN18" s="4"/>
-      <c r="AO18" s="4"/>
-      <c r="AP18" s="4"/>
-      <c r="AQ18" s="4"/>
-      <c r="AR18" s="4"/>
-      <c r="AS18" s="4"/>
-      <c r="AT18" s="4"/>
-      <c r="AU18" s="4"/>
-      <c r="AV18" s="4"/>
-      <c r="AW18" s="4"/>
-      <c r="AX18" s="4"/>
-      <c r="AY18" s="4"/>
-      <c r="AZ18" s="4"/>
-      <c r="BA18" s="4"/>
-      <c r="BB18" s="4"/>
-      <c r="BC18" s="4"/>
-      <c r="BD18" s="4"/>
-      <c r="BE18" s="4"/>
-      <c r="BF18" s="4"/>
-      <c r="BG18" s="4"/>
-      <c r="BH18" s="4"/>
-      <c r="BI18" s="4"/>
-      <c r="BJ18" s="4"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="3"/>
+      <c r="AO18" s="3"/>
+      <c r="AP18" s="3"/>
+      <c r="AQ18" s="3"/>
+      <c r="AR18" s="3"/>
+      <c r="AS18" s="3"/>
+      <c r="AT18" s="3"/>
+      <c r="AU18" s="3"/>
+      <c r="AV18" s="3"/>
+      <c r="AW18" s="3"/>
+      <c r="AX18" s="3"/>
+      <c r="AY18" s="3"/>
+      <c r="AZ18" s="3"/>
+      <c r="BA18" s="3"/>
+      <c r="BB18" s="3"/>
+      <c r="BC18" s="3"/>
+      <c r="BD18" s="3"/>
+      <c r="BE18" s="3"/>
+      <c r="BF18" s="3"/>
+      <c r="BG18" s="3"/>
+      <c r="BH18" s="3"/>
+      <c r="BI18" s="3"/>
+      <c r="BJ18" s="3"/>
     </row>
     <row r="19" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -4351,35 +4351,35 @@
       <c r="AF19">
         <v>0</v>
       </c>
-      <c r="AH19" s="4"/>
-      <c r="AI19" s="4"/>
-      <c r="AJ19" s="4"/>
-      <c r="AK19" s="4"/>
-      <c r="AL19" s="4"/>
-      <c r="AM19" s="4"/>
-      <c r="AN19" s="4"/>
-      <c r="AO19" s="4"/>
-      <c r="AP19" s="4"/>
-      <c r="AQ19" s="4"/>
-      <c r="AR19" s="4"/>
-      <c r="AS19" s="4"/>
-      <c r="AT19" s="4"/>
-      <c r="AU19" s="4"/>
-      <c r="AV19" s="4"/>
-      <c r="AW19" s="4"/>
-      <c r="AX19" s="4"/>
-      <c r="AY19" s="4"/>
-      <c r="AZ19" s="4"/>
-      <c r="BA19" s="4"/>
-      <c r="BB19" s="4"/>
-      <c r="BC19" s="4"/>
-      <c r="BD19" s="4"/>
-      <c r="BE19" s="4"/>
-      <c r="BF19" s="4"/>
-      <c r="BG19" s="4"/>
-      <c r="BH19" s="4"/>
-      <c r="BI19" s="4"/>
-      <c r="BJ19" s="4"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="3"/>
+      <c r="AN19" s="3"/>
+      <c r="AO19" s="3"/>
+      <c r="AP19" s="3"/>
+      <c r="AQ19" s="3"/>
+      <c r="AR19" s="3"/>
+      <c r="AS19" s="3"/>
+      <c r="AT19" s="3"/>
+      <c r="AU19" s="3"/>
+      <c r="AV19" s="3"/>
+      <c r="AW19" s="3"/>
+      <c r="AX19" s="3"/>
+      <c r="AY19" s="3"/>
+      <c r="AZ19" s="3"/>
+      <c r="BA19" s="3"/>
+      <c r="BB19" s="3"/>
+      <c r="BC19" s="3"/>
+      <c r="BD19" s="3"/>
+      <c r="BE19" s="3"/>
+      <c r="BF19" s="3"/>
+      <c r="BG19" s="3"/>
+      <c r="BH19" s="3"/>
+      <c r="BI19" s="3"/>
+      <c r="BJ19" s="3"/>
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -4478,35 +4478,35 @@
       <c r="AF20">
         <v>0</v>
       </c>
-      <c r="AH20" s="4"/>
-      <c r="AI20" s="4"/>
-      <c r="AJ20" s="4"/>
-      <c r="AK20" s="4"/>
-      <c r="AL20" s="4"/>
-      <c r="AM20" s="4"/>
-      <c r="AN20" s="4"/>
-      <c r="AO20" s="4"/>
-      <c r="AP20" s="4"/>
-      <c r="AQ20" s="4"/>
-      <c r="AR20" s="4"/>
-      <c r="AS20" s="4"/>
-      <c r="AT20" s="4"/>
-      <c r="AU20" s="4"/>
-      <c r="AV20" s="4"/>
-      <c r="AW20" s="4"/>
-      <c r="AX20" s="4"/>
-      <c r="AY20" s="4"/>
-      <c r="AZ20" s="4"/>
-      <c r="BA20" s="4"/>
-      <c r="BB20" s="4"/>
-      <c r="BC20" s="4"/>
-      <c r="BD20" s="4"/>
-      <c r="BE20" s="4"/>
-      <c r="BF20" s="4"/>
-      <c r="BG20" s="4"/>
-      <c r="BH20" s="4"/>
-      <c r="BI20" s="4"/>
-      <c r="BJ20" s="4"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="3"/>
+      <c r="AN20" s="3"/>
+      <c r="AO20" s="3"/>
+      <c r="AP20" s="3"/>
+      <c r="AQ20" s="3"/>
+      <c r="AR20" s="3"/>
+      <c r="AS20" s="3"/>
+      <c r="AT20" s="3"/>
+      <c r="AU20" s="3"/>
+      <c r="AV20" s="3"/>
+      <c r="AW20" s="3"/>
+      <c r="AX20" s="3"/>
+      <c r="AY20" s="3"/>
+      <c r="AZ20" s="3"/>
+      <c r="BA20" s="3"/>
+      <c r="BB20" s="3"/>
+      <c r="BC20" s="3"/>
+      <c r="BD20" s="3"/>
+      <c r="BE20" s="3"/>
+      <c r="BF20" s="3"/>
+      <c r="BG20" s="3"/>
+      <c r="BH20" s="3"/>
+      <c r="BI20" s="3"/>
+      <c r="BJ20" s="3"/>
     </row>
     <row r="21" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -4605,35 +4605,35 @@
       <c r="AF21">
         <v>0.27549145180915802</v>
       </c>
-      <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
-      <c r="AJ21" s="4"/>
-      <c r="AK21" s="4"/>
-      <c r="AL21" s="4"/>
-      <c r="AM21" s="4"/>
-      <c r="AN21" s="4"/>
-      <c r="AO21" s="4"/>
-      <c r="AP21" s="4"/>
-      <c r="AQ21" s="4"/>
-      <c r="AR21" s="4"/>
-      <c r="AS21" s="4"/>
-      <c r="AT21" s="4"/>
-      <c r="AU21" s="4"/>
-      <c r="AV21" s="4"/>
-      <c r="AW21" s="4"/>
-      <c r="AX21" s="4"/>
-      <c r="AY21" s="4"/>
-      <c r="AZ21" s="4"/>
-      <c r="BA21" s="4"/>
-      <c r="BB21" s="4"/>
-      <c r="BC21" s="4"/>
-      <c r="BD21" s="4"/>
-      <c r="BE21" s="4"/>
-      <c r="BF21" s="4"/>
-      <c r="BG21" s="4"/>
-      <c r="BH21" s="4"/>
-      <c r="BI21" s="4"/>
-      <c r="BJ21" s="4"/>
+      <c r="AH21" s="3"/>
+      <c r="AI21" s="3"/>
+      <c r="AJ21" s="3"/>
+      <c r="AK21" s="3"/>
+      <c r="AL21" s="3"/>
+      <c r="AM21" s="3"/>
+      <c r="AN21" s="3"/>
+      <c r="AO21" s="3"/>
+      <c r="AP21" s="3"/>
+      <c r="AQ21" s="3"/>
+      <c r="AR21" s="3"/>
+      <c r="AS21" s="3"/>
+      <c r="AT21" s="3"/>
+      <c r="AU21" s="3"/>
+      <c r="AV21" s="3"/>
+      <c r="AW21" s="3"/>
+      <c r="AX21" s="3"/>
+      <c r="AY21" s="3"/>
+      <c r="AZ21" s="3"/>
+      <c r="BA21" s="3"/>
+      <c r="BB21" s="3"/>
+      <c r="BC21" s="3"/>
+      <c r="BD21" s="3"/>
+      <c r="BE21" s="3"/>
+      <c r="BF21" s="3"/>
+      <c r="BG21" s="3"/>
+      <c r="BH21" s="3"/>
+      <c r="BI21" s="3"/>
+      <c r="BJ21" s="3"/>
     </row>
     <row r="22" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -4732,35 +4732,35 @@
       <c r="AF22">
         <v>0.174856850144092</v>
       </c>
-      <c r="AH22" s="4"/>
-      <c r="AI22" s="4"/>
-      <c r="AJ22" s="4"/>
-      <c r="AK22" s="4"/>
-      <c r="AL22" s="4"/>
-      <c r="AM22" s="4"/>
-      <c r="AN22" s="4"/>
-      <c r="AO22" s="4"/>
-      <c r="AP22" s="4"/>
-      <c r="AQ22" s="4"/>
-      <c r="AR22" s="4"/>
-      <c r="AS22" s="4"/>
-      <c r="AT22" s="4"/>
-      <c r="AU22" s="4"/>
-      <c r="AV22" s="4"/>
-      <c r="AW22" s="4"/>
-      <c r="AX22" s="4"/>
-      <c r="AY22" s="4"/>
-      <c r="AZ22" s="4"/>
-      <c r="BA22" s="4"/>
-      <c r="BB22" s="4"/>
-      <c r="BC22" s="4"/>
-      <c r="BD22" s="4"/>
-      <c r="BE22" s="4"/>
-      <c r="BF22" s="4"/>
-      <c r="BG22" s="4"/>
-      <c r="BH22" s="4"/>
-      <c r="BI22" s="4"/>
-      <c r="BJ22" s="4"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3"/>
+      <c r="AN22" s="3"/>
+      <c r="AO22" s="3"/>
+      <c r="AP22" s="3"/>
+      <c r="AQ22" s="3"/>
+      <c r="AR22" s="3"/>
+      <c r="AS22" s="3"/>
+      <c r="AT22" s="3"/>
+      <c r="AU22" s="3"/>
+      <c r="AV22" s="3"/>
+      <c r="AW22" s="3"/>
+      <c r="AX22" s="3"/>
+      <c r="AY22" s="3"/>
+      <c r="AZ22" s="3"/>
+      <c r="BA22" s="3"/>
+      <c r="BB22" s="3"/>
+      <c r="BC22" s="3"/>
+      <c r="BD22" s="3"/>
+      <c r="BE22" s="3"/>
+      <c r="BF22" s="3"/>
+      <c r="BG22" s="3"/>
+      <c r="BH22" s="3"/>
+      <c r="BI22" s="3"/>
+      <c r="BJ22" s="3"/>
     </row>
     <row r="23" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -4859,35 +4859,35 @@
       <c r="AF23">
         <v>0</v>
       </c>
-      <c r="AH23" s="4"/>
-      <c r="AI23" s="4"/>
-      <c r="AJ23" s="4"/>
-      <c r="AK23" s="4"/>
-      <c r="AL23" s="4"/>
-      <c r="AM23" s="4"/>
-      <c r="AN23" s="4"/>
-      <c r="AO23" s="4"/>
-      <c r="AP23" s="4"/>
-      <c r="AQ23" s="4"/>
-      <c r="AR23" s="4"/>
-      <c r="AS23" s="4"/>
-      <c r="AT23" s="4"/>
-      <c r="AU23" s="4"/>
-      <c r="AV23" s="4"/>
-      <c r="AW23" s="4"/>
-      <c r="AX23" s="4"/>
-      <c r="AY23" s="4"/>
-      <c r="AZ23" s="4"/>
-      <c r="BA23" s="4"/>
-      <c r="BB23" s="4"/>
-      <c r="BC23" s="4"/>
-      <c r="BD23" s="4"/>
-      <c r="BE23" s="4"/>
-      <c r="BF23" s="4"/>
-      <c r="BG23" s="4"/>
-      <c r="BH23" s="4"/>
-      <c r="BI23" s="4"/>
-      <c r="BJ23" s="4"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+      <c r="AT23" s="3"/>
+      <c r="AU23" s="3"/>
+      <c r="AV23" s="3"/>
+      <c r="AW23" s="3"/>
+      <c r="AX23" s="3"/>
+      <c r="AY23" s="3"/>
+      <c r="AZ23" s="3"/>
+      <c r="BA23" s="3"/>
+      <c r="BB23" s="3"/>
+      <c r="BC23" s="3"/>
+      <c r="BD23" s="3"/>
+      <c r="BE23" s="3"/>
+      <c r="BF23" s="3"/>
+      <c r="BG23" s="3"/>
+      <c r="BH23" s="3"/>
+      <c r="BI23" s="3"/>
+      <c r="BJ23" s="3"/>
     </row>
     <row r="24" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -4986,35 +4986,35 @@
       <c r="AF24">
         <v>0</v>
       </c>
-      <c r="AH24" s="4"/>
-      <c r="AI24" s="4"/>
-      <c r="AJ24" s="4"/>
-      <c r="AK24" s="4"/>
-      <c r="AL24" s="4"/>
-      <c r="AM24" s="4"/>
-      <c r="AN24" s="4"/>
-      <c r="AO24" s="4"/>
-      <c r="AP24" s="4"/>
-      <c r="AQ24" s="4"/>
-      <c r="AR24" s="4"/>
-      <c r="AS24" s="4"/>
-      <c r="AT24" s="4"/>
-      <c r="AU24" s="4"/>
-      <c r="AV24" s="4"/>
-      <c r="AW24" s="4"/>
-      <c r="AX24" s="4"/>
-      <c r="AY24" s="4"/>
-      <c r="AZ24" s="4"/>
-      <c r="BA24" s="4"/>
-      <c r="BB24" s="4"/>
-      <c r="BC24" s="4"/>
-      <c r="BD24" s="4"/>
-      <c r="BE24" s="4"/>
-      <c r="BF24" s="4"/>
-      <c r="BG24" s="4"/>
-      <c r="BH24" s="4"/>
-      <c r="BI24" s="4"/>
-      <c r="BJ24" s="4"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="3"/>
+      <c r="AO24" s="3"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+      <c r="AT24" s="3"/>
+      <c r="AU24" s="3"/>
+      <c r="AV24" s="3"/>
+      <c r="AW24" s="3"/>
+      <c r="AX24" s="3"/>
+      <c r="AY24" s="3"/>
+      <c r="AZ24" s="3"/>
+      <c r="BA24" s="3"/>
+      <c r="BB24" s="3"/>
+      <c r="BC24" s="3"/>
+      <c r="BD24" s="3"/>
+      <c r="BE24" s="3"/>
+      <c r="BF24" s="3"/>
+      <c r="BG24" s="3"/>
+      <c r="BH24" s="3"/>
+      <c r="BI24" s="3"/>
+      <c r="BJ24" s="3"/>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -5113,35 +5113,35 @@
       <c r="AF25">
         <v>0</v>
       </c>
-      <c r="AH25" s="4"/>
-      <c r="AI25" s="4"/>
-      <c r="AJ25" s="4"/>
-      <c r="AK25" s="4"/>
-      <c r="AL25" s="4"/>
-      <c r="AM25" s="4"/>
-      <c r="AN25" s="4"/>
-      <c r="AO25" s="4"/>
-      <c r="AP25" s="4"/>
-      <c r="AQ25" s="4"/>
-      <c r="AR25" s="4"/>
-      <c r="AS25" s="4"/>
-      <c r="AT25" s="4"/>
-      <c r="AU25" s="4"/>
-      <c r="AV25" s="4"/>
-      <c r="AW25" s="4"/>
-      <c r="AX25" s="4"/>
-      <c r="AY25" s="4"/>
-      <c r="AZ25" s="4"/>
-      <c r="BA25" s="4"/>
-      <c r="BB25" s="4"/>
-      <c r="BC25" s="4"/>
-      <c r="BD25" s="4"/>
-      <c r="BE25" s="4"/>
-      <c r="BF25" s="4"/>
-      <c r="BG25" s="4"/>
-      <c r="BH25" s="4"/>
-      <c r="BI25" s="4"/>
-      <c r="BJ25" s="4"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="3"/>
+      <c r="AO25" s="3"/>
+      <c r="AP25" s="3"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="3"/>
+      <c r="AU25" s="3"/>
+      <c r="AV25" s="3"/>
+      <c r="AW25" s="3"/>
+      <c r="AX25" s="3"/>
+      <c r="AY25" s="3"/>
+      <c r="AZ25" s="3"/>
+      <c r="BA25" s="3"/>
+      <c r="BB25" s="3"/>
+      <c r="BC25" s="3"/>
+      <c r="BD25" s="3"/>
+      <c r="BE25" s="3"/>
+      <c r="BF25" s="3"/>
+      <c r="BG25" s="3"/>
+      <c r="BH25" s="3"/>
+      <c r="BI25" s="3"/>
+      <c r="BJ25" s="3"/>
     </row>
     <row r="26" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -5240,35 +5240,35 @@
       <c r="AF26">
         <v>0</v>
       </c>
-      <c r="AH26" s="4"/>
-      <c r="AI26" s="4"/>
-      <c r="AJ26" s="4"/>
-      <c r="AK26" s="4"/>
-      <c r="AL26" s="4"/>
-      <c r="AM26" s="4"/>
-      <c r="AN26" s="4"/>
-      <c r="AO26" s="4"/>
-      <c r="AP26" s="4"/>
-      <c r="AQ26" s="4"/>
-      <c r="AR26" s="4"/>
-      <c r="AS26" s="4"/>
-      <c r="AT26" s="4"/>
-      <c r="AU26" s="4"/>
-      <c r="AV26" s="4"/>
-      <c r="AW26" s="4"/>
-      <c r="AX26" s="4"/>
-      <c r="AY26" s="4"/>
-      <c r="AZ26" s="4"/>
-      <c r="BA26" s="4"/>
-      <c r="BB26" s="4"/>
-      <c r="BC26" s="4"/>
-      <c r="BD26" s="4"/>
-      <c r="BE26" s="4"/>
-      <c r="BF26" s="4"/>
-      <c r="BG26" s="4"/>
-      <c r="BH26" s="4"/>
-      <c r="BI26" s="4"/>
-      <c r="BJ26" s="4"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="3"/>
+      <c r="AN26" s="3"/>
+      <c r="AO26" s="3"/>
+      <c r="AP26" s="3"/>
+      <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
+      <c r="AS26" s="3"/>
+      <c r="AT26" s="3"/>
+      <c r="AU26" s="3"/>
+      <c r="AV26" s="3"/>
+      <c r="AW26" s="3"/>
+      <c r="AX26" s="3"/>
+      <c r="AY26" s="3"/>
+      <c r="AZ26" s="3"/>
+      <c r="BA26" s="3"/>
+      <c r="BB26" s="3"/>
+      <c r="BC26" s="3"/>
+      <c r="BD26" s="3"/>
+      <c r="BE26" s="3"/>
+      <c r="BF26" s="3"/>
+      <c r="BG26" s="3"/>
+      <c r="BH26" s="3"/>
+      <c r="BI26" s="3"/>
+      <c r="BJ26" s="3"/>
     </row>
     <row r="27" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -5367,35 +5367,35 @@
       <c r="AF27">
         <v>0.14899256772334299</v>
       </c>
-      <c r="AH27" s="4"/>
-      <c r="AI27" s="4"/>
-      <c r="AJ27" s="4"/>
-      <c r="AK27" s="4"/>
-      <c r="AL27" s="4"/>
-      <c r="AM27" s="4"/>
-      <c r="AN27" s="4"/>
-      <c r="AO27" s="4"/>
-      <c r="AP27" s="4"/>
-      <c r="AQ27" s="4"/>
-      <c r="AR27" s="4"/>
-      <c r="AS27" s="4"/>
-      <c r="AT27" s="4"/>
-      <c r="AU27" s="4"/>
-      <c r="AV27" s="4"/>
-      <c r="AW27" s="4"/>
-      <c r="AX27" s="4"/>
-      <c r="AY27" s="4"/>
-      <c r="AZ27" s="4"/>
-      <c r="BA27" s="4"/>
-      <c r="BB27" s="4"/>
-      <c r="BC27" s="4"/>
-      <c r="BD27" s="4"/>
-      <c r="BE27" s="4"/>
-      <c r="BF27" s="4"/>
-      <c r="BG27" s="4"/>
-      <c r="BH27" s="4"/>
-      <c r="BI27" s="4"/>
-      <c r="BJ27" s="4"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3"/>
+      <c r="AN27" s="3"/>
+      <c r="AO27" s="3"/>
+      <c r="AP27" s="3"/>
+      <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="3"/>
+      <c r="AT27" s="3"/>
+      <c r="AU27" s="3"/>
+      <c r="AV27" s="3"/>
+      <c r="AW27" s="3"/>
+      <c r="AX27" s="3"/>
+      <c r="AY27" s="3"/>
+      <c r="AZ27" s="3"/>
+      <c r="BA27" s="3"/>
+      <c r="BB27" s="3"/>
+      <c r="BC27" s="3"/>
+      <c r="BD27" s="3"/>
+      <c r="BE27" s="3"/>
+      <c r="BF27" s="3"/>
+      <c r="BG27" s="3"/>
+      <c r="BH27" s="3"/>
+      <c r="BI27" s="3"/>
+      <c r="BJ27" s="3"/>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -5494,35 +5494,35 @@
       <c r="AF28">
         <v>0.375250401857189</v>
       </c>
-      <c r="AH28" s="4"/>
-      <c r="AI28" s="4"/>
-      <c r="AJ28" s="4"/>
-      <c r="AK28" s="4"/>
-      <c r="AL28" s="4"/>
-      <c r="AM28" s="4"/>
-      <c r="AN28" s="4"/>
-      <c r="AO28" s="4"/>
-      <c r="AP28" s="4"/>
-      <c r="AQ28" s="4"/>
-      <c r="AR28" s="4"/>
-      <c r="AS28" s="4"/>
-      <c r="AT28" s="4"/>
-      <c r="AU28" s="4"/>
-      <c r="AV28" s="4"/>
-      <c r="AW28" s="4"/>
-      <c r="AX28" s="4"/>
-      <c r="AY28" s="4"/>
-      <c r="AZ28" s="4"/>
-      <c r="BA28" s="4"/>
-      <c r="BB28" s="4"/>
-      <c r="BC28" s="4"/>
-      <c r="BD28" s="4"/>
-      <c r="BE28" s="4"/>
-      <c r="BF28" s="4"/>
-      <c r="BG28" s="4"/>
-      <c r="BH28" s="4"/>
-      <c r="BI28" s="4"/>
-      <c r="BJ28" s="4"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="3"/>
+      <c r="AN28" s="3"/>
+      <c r="AO28" s="3"/>
+      <c r="AP28" s="3"/>
+      <c r="AQ28" s="3"/>
+      <c r="AR28" s="3"/>
+      <c r="AS28" s="3"/>
+      <c r="AT28" s="3"/>
+      <c r="AU28" s="3"/>
+      <c r="AV28" s="3"/>
+      <c r="AW28" s="3"/>
+      <c r="AX28" s="3"/>
+      <c r="AY28" s="3"/>
+      <c r="AZ28" s="3"/>
+      <c r="BA28" s="3"/>
+      <c r="BB28" s="3"/>
+      <c r="BC28" s="3"/>
+      <c r="BD28" s="3"/>
+      <c r="BE28" s="3"/>
+      <c r="BF28" s="3"/>
+      <c r="BG28" s="3"/>
+      <c r="BH28" s="3"/>
+      <c r="BI28" s="3"/>
+      <c r="BJ28" s="3"/>
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -5621,35 +5621,35 @@
       <c r="AF29">
         <v>0</v>
       </c>
-      <c r="AH29" s="4"/>
-      <c r="AI29" s="4"/>
-      <c r="AJ29" s="4"/>
-      <c r="AK29" s="4"/>
-      <c r="AL29" s="4"/>
-      <c r="AM29" s="4"/>
-      <c r="AN29" s="4"/>
-      <c r="AO29" s="4"/>
-      <c r="AP29" s="4"/>
-      <c r="AQ29" s="4"/>
-      <c r="AR29" s="4"/>
-      <c r="AS29" s="4"/>
-      <c r="AT29" s="4"/>
-      <c r="AU29" s="4"/>
-      <c r="AV29" s="4"/>
-      <c r="AW29" s="4"/>
-      <c r="AX29" s="4"/>
-      <c r="AY29" s="4"/>
-      <c r="AZ29" s="4"/>
-      <c r="BA29" s="4"/>
-      <c r="BB29" s="4"/>
-      <c r="BC29" s="4"/>
-      <c r="BD29" s="4"/>
-      <c r="BE29" s="4"/>
-      <c r="BF29" s="4"/>
-      <c r="BG29" s="4"/>
-      <c r="BH29" s="4"/>
-      <c r="BI29" s="4"/>
-      <c r="BJ29" s="4"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="3"/>
+      <c r="AN29" s="3"/>
+      <c r="AO29" s="3"/>
+      <c r="AP29" s="3"/>
+      <c r="AQ29" s="3"/>
+      <c r="AR29" s="3"/>
+      <c r="AS29" s="3"/>
+      <c r="AT29" s="3"/>
+      <c r="AU29" s="3"/>
+      <c r="AV29" s="3"/>
+      <c r="AW29" s="3"/>
+      <c r="AX29" s="3"/>
+      <c r="AY29" s="3"/>
+      <c r="AZ29" s="3"/>
+      <c r="BA29" s="3"/>
+      <c r="BB29" s="3"/>
+      <c r="BC29" s="3"/>
+      <c r="BD29" s="3"/>
+      <c r="BE29" s="3"/>
+      <c r="BF29" s="3"/>
+      <c r="BG29" s="3"/>
+      <c r="BH29" s="3"/>
+      <c r="BI29" s="3"/>
+      <c r="BJ29" s="3"/>
     </row>
     <row r="30" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -5748,35 +5748,35 @@
       <c r="AF30">
         <v>0</v>
       </c>
-      <c r="AH30" s="4"/>
-      <c r="AI30" s="4"/>
-      <c r="AJ30" s="4"/>
-      <c r="AK30" s="4"/>
-      <c r="AL30" s="4"/>
-      <c r="AM30" s="4"/>
-      <c r="AN30" s="4"/>
-      <c r="AO30" s="4"/>
-      <c r="AP30" s="4"/>
-      <c r="AQ30" s="4"/>
-      <c r="AR30" s="4"/>
-      <c r="AS30" s="4"/>
-      <c r="AT30" s="4"/>
-      <c r="AU30" s="4"/>
-      <c r="AV30" s="4"/>
-      <c r="AW30" s="4"/>
-      <c r="AX30" s="4"/>
-      <c r="AY30" s="4"/>
-      <c r="AZ30" s="4"/>
-      <c r="BA30" s="4"/>
-      <c r="BB30" s="4"/>
-      <c r="BC30" s="4"/>
-      <c r="BD30" s="4"/>
-      <c r="BE30" s="4"/>
-      <c r="BF30" s="4"/>
-      <c r="BG30" s="4"/>
-      <c r="BH30" s="4"/>
-      <c r="BI30" s="4"/>
-      <c r="BJ30" s="4"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="3"/>
+      <c r="AM30" s="3"/>
+      <c r="AN30" s="3"/>
+      <c r="AO30" s="3"/>
+      <c r="AP30" s="3"/>
+      <c r="AQ30" s="3"/>
+      <c r="AR30" s="3"/>
+      <c r="AS30" s="3"/>
+      <c r="AT30" s="3"/>
+      <c r="AU30" s="3"/>
+      <c r="AV30" s="3"/>
+      <c r="AW30" s="3"/>
+      <c r="AX30" s="3"/>
+      <c r="AY30" s="3"/>
+      <c r="AZ30" s="3"/>
+      <c r="BA30" s="3"/>
+      <c r="BB30" s="3"/>
+      <c r="BC30" s="3"/>
+      <c r="BD30" s="3"/>
+      <c r="BE30" s="3"/>
+      <c r="BF30" s="3"/>
+      <c r="BG30" s="3"/>
+      <c r="BH30" s="3"/>
+      <c r="BI30" s="3"/>
+      <c r="BJ30" s="3"/>
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -5875,35 +5875,35 @@
       <c r="AF31">
         <v>7.9644032981107907E-2</v>
       </c>
-      <c r="AH31" s="4"/>
-      <c r="AI31" s="4"/>
-      <c r="AJ31" s="4"/>
-      <c r="AK31" s="4"/>
-      <c r="AL31" s="4"/>
-      <c r="AM31" s="4"/>
-      <c r="AN31" s="4"/>
-      <c r="AO31" s="4"/>
-      <c r="AP31" s="4"/>
-      <c r="AQ31" s="4"/>
-      <c r="AR31" s="4"/>
-      <c r="AS31" s="4"/>
-      <c r="AT31" s="4"/>
-      <c r="AU31" s="4"/>
-      <c r="AV31" s="4"/>
-      <c r="AW31" s="4"/>
-      <c r="AX31" s="4"/>
-      <c r="AY31" s="4"/>
-      <c r="AZ31" s="4"/>
-      <c r="BA31" s="4"/>
-      <c r="BB31" s="4"/>
-      <c r="BC31" s="4"/>
-      <c r="BD31" s="4"/>
-      <c r="BE31" s="4"/>
-      <c r="BF31" s="4"/>
-      <c r="BG31" s="4"/>
-      <c r="BH31" s="4"/>
-      <c r="BI31" s="4"/>
-      <c r="BJ31" s="4"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
+      <c r="AN31" s="3"/>
+      <c r="AO31" s="3"/>
+      <c r="AP31" s="3"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="3"/>
+      <c r="AU31" s="3"/>
+      <c r="AV31" s="3"/>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="3"/>
+      <c r="AY31" s="3"/>
+      <c r="AZ31" s="3"/>
+      <c r="BA31" s="3"/>
+      <c r="BB31" s="3"/>
+      <c r="BC31" s="3"/>
+      <c r="BD31" s="3"/>
+      <c r="BE31" s="3"/>
+      <c r="BF31" s="3"/>
+      <c r="BG31" s="3"/>
+      <c r="BH31" s="3"/>
+      <c r="BI31" s="3"/>
+      <c r="BJ31" s="3"/>
     </row>
     <row r="32" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -6002,35 +6002,35 @@
       <c r="AF32">
         <v>0.24621114217098899</v>
       </c>
-      <c r="AH32" s="4"/>
-      <c r="AI32" s="4"/>
-      <c r="AJ32" s="4"/>
-      <c r="AK32" s="4"/>
-      <c r="AL32" s="4"/>
-      <c r="AM32" s="4"/>
-      <c r="AN32" s="4"/>
-      <c r="AO32" s="4"/>
-      <c r="AP32" s="4"/>
-      <c r="AQ32" s="4"/>
-      <c r="AR32" s="4"/>
-      <c r="AS32" s="4"/>
-      <c r="AT32" s="4"/>
-      <c r="AU32" s="4"/>
-      <c r="AV32" s="4"/>
-      <c r="AW32" s="4"/>
-      <c r="AX32" s="4"/>
-      <c r="AY32" s="4"/>
-      <c r="AZ32" s="4"/>
-      <c r="BA32" s="4"/>
-      <c r="BB32" s="4"/>
-      <c r="BC32" s="4"/>
-      <c r="BD32" s="4"/>
-      <c r="BE32" s="4"/>
-      <c r="BF32" s="4"/>
-      <c r="BG32" s="4"/>
-      <c r="BH32" s="4"/>
-      <c r="BI32" s="4"/>
-      <c r="BJ32" s="4"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
+      <c r="AM32" s="3"/>
+      <c r="AN32" s="3"/>
+      <c r="AO32" s="3"/>
+      <c r="AP32" s="3"/>
+      <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
+      <c r="AS32" s="3"/>
+      <c r="AT32" s="3"/>
+      <c r="AU32" s="3"/>
+      <c r="AV32" s="3"/>
+      <c r="AW32" s="3"/>
+      <c r="AX32" s="3"/>
+      <c r="AY32" s="3"/>
+      <c r="AZ32" s="3"/>
+      <c r="BA32" s="3"/>
+      <c r="BB32" s="3"/>
+      <c r="BC32" s="3"/>
+      <c r="BD32" s="3"/>
+      <c r="BE32" s="3"/>
+      <c r="BF32" s="3"/>
+      <c r="BG32" s="3"/>
+      <c r="BH32" s="3"/>
+      <c r="BI32" s="3"/>
+      <c r="BJ32" s="3"/>
     </row>
     <row r="33" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -6129,35 +6129,35 @@
       <c r="AF33">
         <v>1.6358830137688101</v>
       </c>
-      <c r="AH33" s="4"/>
-      <c r="AI33" s="4"/>
-      <c r="AJ33" s="4"/>
-      <c r="AK33" s="4"/>
-      <c r="AL33" s="4"/>
-      <c r="AM33" s="4"/>
-      <c r="AN33" s="4"/>
-      <c r="AO33" s="4"/>
-      <c r="AP33" s="4"/>
-      <c r="AQ33" s="4"/>
-      <c r="AR33" s="4"/>
-      <c r="AS33" s="4"/>
-      <c r="AT33" s="4"/>
-      <c r="AU33" s="4"/>
-      <c r="AV33" s="4"/>
-      <c r="AW33" s="4"/>
-      <c r="AX33" s="4"/>
-      <c r="AY33" s="4"/>
-      <c r="AZ33" s="4"/>
-      <c r="BA33" s="4"/>
-      <c r="BB33" s="4"/>
-      <c r="BC33" s="4"/>
-      <c r="BD33" s="4"/>
-      <c r="BE33" s="4"/>
-      <c r="BF33" s="4"/>
-      <c r="BG33" s="4"/>
-      <c r="BH33" s="4"/>
-      <c r="BI33" s="4"/>
-      <c r="BJ33" s="4"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="3"/>
+      <c r="AM33" s="3"/>
+      <c r="AN33" s="3"/>
+      <c r="AO33" s="3"/>
+      <c r="AP33" s="3"/>
+      <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
+      <c r="AS33" s="3"/>
+      <c r="AT33" s="3"/>
+      <c r="AU33" s="3"/>
+      <c r="AV33" s="3"/>
+      <c r="AW33" s="3"/>
+      <c r="AX33" s="3"/>
+      <c r="AY33" s="3"/>
+      <c r="AZ33" s="3"/>
+      <c r="BA33" s="3"/>
+      <c r="BB33" s="3"/>
+      <c r="BC33" s="3"/>
+      <c r="BD33" s="3"/>
+      <c r="BE33" s="3"/>
+      <c r="BF33" s="3"/>
+      <c r="BG33" s="3"/>
+      <c r="BH33" s="3"/>
+      <c r="BI33" s="3"/>
+      <c r="BJ33" s="3"/>
     </row>
     <row r="34" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -6256,35 +6256,35 @@
       <c r="AF34">
         <v>0.39839088664745398</v>
       </c>
-      <c r="AH34" s="4"/>
-      <c r="AI34" s="4"/>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="4"/>
-      <c r="AL34" s="4"/>
-      <c r="AM34" s="4"/>
-      <c r="AN34" s="4"/>
-      <c r="AO34" s="4"/>
-      <c r="AP34" s="4"/>
-      <c r="AQ34" s="4"/>
-      <c r="AR34" s="4"/>
-      <c r="AS34" s="4"/>
-      <c r="AT34" s="4"/>
-      <c r="AU34" s="4"/>
-      <c r="AV34" s="4"/>
-      <c r="AW34" s="4"/>
-      <c r="AX34" s="4"/>
-      <c r="AY34" s="4"/>
-      <c r="AZ34" s="4"/>
-      <c r="BA34" s="4"/>
-      <c r="BB34" s="4"/>
-      <c r="BC34" s="4"/>
-      <c r="BD34" s="4"/>
-      <c r="BE34" s="4"/>
-      <c r="BF34" s="4"/>
-      <c r="BG34" s="4"/>
-      <c r="BH34" s="4"/>
-      <c r="BI34" s="4"/>
-      <c r="BJ34" s="4"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3"/>
+      <c r="AL34" s="3"/>
+      <c r="AM34" s="3"/>
+      <c r="AN34" s="3"/>
+      <c r="AO34" s="3"/>
+      <c r="AP34" s="3"/>
+      <c r="AQ34" s="3"/>
+      <c r="AR34" s="3"/>
+      <c r="AS34" s="3"/>
+      <c r="AT34" s="3"/>
+      <c r="AU34" s="3"/>
+      <c r="AV34" s="3"/>
+      <c r="AW34" s="3"/>
+      <c r="AX34" s="3"/>
+      <c r="AY34" s="3"/>
+      <c r="AZ34" s="3"/>
+      <c r="BA34" s="3"/>
+      <c r="BB34" s="3"/>
+      <c r="BC34" s="3"/>
+      <c r="BD34" s="3"/>
+      <c r="BE34" s="3"/>
+      <c r="BF34" s="3"/>
+      <c r="BG34" s="3"/>
+      <c r="BH34" s="3"/>
+      <c r="BI34" s="3"/>
+      <c r="BJ34" s="3"/>
     </row>
     <row r="35" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -6383,35 +6383,35 @@
       <c r="AF35">
         <v>1.3968985091258399</v>
       </c>
-      <c r="AH35" s="4"/>
-      <c r="AI35" s="4"/>
-      <c r="AJ35" s="4"/>
-      <c r="AK35" s="4"/>
-      <c r="AL35" s="4"/>
-      <c r="AM35" s="4"/>
-      <c r="AN35" s="4"/>
-      <c r="AO35" s="4"/>
-      <c r="AP35" s="4"/>
-      <c r="AQ35" s="4"/>
-      <c r="AR35" s="4"/>
-      <c r="AS35" s="4"/>
-      <c r="AT35" s="4"/>
-      <c r="AU35" s="4"/>
-      <c r="AV35" s="4"/>
-      <c r="AW35" s="4"/>
-      <c r="AX35" s="4"/>
-      <c r="AY35" s="4"/>
-      <c r="AZ35" s="4"/>
-      <c r="BA35" s="4"/>
-      <c r="BB35" s="4"/>
-      <c r="BC35" s="4"/>
-      <c r="BD35" s="4"/>
-      <c r="BE35" s="4"/>
-      <c r="BF35" s="4"/>
-      <c r="BG35" s="4"/>
-      <c r="BH35" s="4"/>
-      <c r="BI35" s="4"/>
-      <c r="BJ35" s="4"/>
+      <c r="AH35" s="3"/>
+      <c r="AI35" s="3"/>
+      <c r="AJ35" s="3"/>
+      <c r="AK35" s="3"/>
+      <c r="AL35" s="3"/>
+      <c r="AM35" s="3"/>
+      <c r="AN35" s="3"/>
+      <c r="AO35" s="3"/>
+      <c r="AP35" s="3"/>
+      <c r="AQ35" s="3"/>
+      <c r="AR35" s="3"/>
+      <c r="AS35" s="3"/>
+      <c r="AT35" s="3"/>
+      <c r="AU35" s="3"/>
+      <c r="AV35" s="3"/>
+      <c r="AW35" s="3"/>
+      <c r="AX35" s="3"/>
+      <c r="AY35" s="3"/>
+      <c r="AZ35" s="3"/>
+      <c r="BA35" s="3"/>
+      <c r="BB35" s="3"/>
+      <c r="BC35" s="3"/>
+      <c r="BD35" s="3"/>
+      <c r="BE35" s="3"/>
+      <c r="BF35" s="3"/>
+      <c r="BG35" s="3"/>
+      <c r="BH35" s="3"/>
+      <c r="BI35" s="3"/>
+      <c r="BJ35" s="3"/>
     </row>
     <row r="36" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -6510,35 +6510,35 @@
       <c r="AF36">
         <v>0.33345074191482499</v>
       </c>
-      <c r="AH36" s="4"/>
-      <c r="AI36" s="4"/>
-      <c r="AJ36" s="4"/>
-      <c r="AK36" s="4"/>
-      <c r="AL36" s="4"/>
-      <c r="AM36" s="4"/>
-      <c r="AN36" s="4"/>
-      <c r="AO36" s="4"/>
-      <c r="AP36" s="4"/>
-      <c r="AQ36" s="4"/>
-      <c r="AR36" s="4"/>
-      <c r="AS36" s="4"/>
-      <c r="AT36" s="4"/>
-      <c r="AU36" s="4"/>
-      <c r="AV36" s="4"/>
-      <c r="AW36" s="4"/>
-      <c r="AX36" s="4"/>
-      <c r="AY36" s="4"/>
-      <c r="AZ36" s="4"/>
-      <c r="BA36" s="4"/>
-      <c r="BB36" s="4"/>
-      <c r="BC36" s="4"/>
-      <c r="BD36" s="4"/>
-      <c r="BE36" s="4"/>
-      <c r="BF36" s="4"/>
-      <c r="BG36" s="4"/>
-      <c r="BH36" s="4"/>
-      <c r="BI36" s="4"/>
-      <c r="BJ36" s="4"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3"/>
+      <c r="AK36" s="3"/>
+      <c r="AL36" s="3"/>
+      <c r="AM36" s="3"/>
+      <c r="AN36" s="3"/>
+      <c r="AO36" s="3"/>
+      <c r="AP36" s="3"/>
+      <c r="AQ36" s="3"/>
+      <c r="AR36" s="3"/>
+      <c r="AS36" s="3"/>
+      <c r="AT36" s="3"/>
+      <c r="AU36" s="3"/>
+      <c r="AV36" s="3"/>
+      <c r="AW36" s="3"/>
+      <c r="AX36" s="3"/>
+      <c r="AY36" s="3"/>
+      <c r="AZ36" s="3"/>
+      <c r="BA36" s="3"/>
+      <c r="BB36" s="3"/>
+      <c r="BC36" s="3"/>
+      <c r="BD36" s="3"/>
+      <c r="BE36" s="3"/>
+      <c r="BF36" s="3"/>
+      <c r="BG36" s="3"/>
+      <c r="BH36" s="3"/>
+      <c r="BI36" s="3"/>
+      <c r="BJ36" s="3"/>
     </row>
     <row r="37" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -6637,35 +6637,35 @@
       <c r="AF37">
         <v>0.30040559301953201</v>
       </c>
-      <c r="AH37" s="4"/>
-      <c r="AI37" s="4"/>
-      <c r="AJ37" s="4"/>
-      <c r="AK37" s="4"/>
-      <c r="AL37" s="4"/>
-      <c r="AM37" s="4"/>
-      <c r="AN37" s="4"/>
-      <c r="AO37" s="4"/>
-      <c r="AP37" s="4"/>
-      <c r="AQ37" s="4"/>
-      <c r="AR37" s="4"/>
-      <c r="AS37" s="4"/>
-      <c r="AT37" s="4"/>
-      <c r="AU37" s="4"/>
-      <c r="AV37" s="4"/>
-      <c r="AW37" s="4"/>
-      <c r="AX37" s="4"/>
-      <c r="AY37" s="4"/>
-      <c r="AZ37" s="4"/>
-      <c r="BA37" s="4"/>
-      <c r="BB37" s="4"/>
-      <c r="BC37" s="4"/>
-      <c r="BD37" s="4"/>
-      <c r="BE37" s="4"/>
-      <c r="BF37" s="4"/>
-      <c r="BG37" s="4"/>
-      <c r="BH37" s="4"/>
-      <c r="BI37" s="4"/>
-      <c r="BJ37" s="4"/>
+      <c r="AH37" s="3"/>
+      <c r="AI37" s="3"/>
+      <c r="AJ37" s="3"/>
+      <c r="AK37" s="3"/>
+      <c r="AL37" s="3"/>
+      <c r="AM37" s="3"/>
+      <c r="AN37" s="3"/>
+      <c r="AO37" s="3"/>
+      <c r="AP37" s="3"/>
+      <c r="AQ37" s="3"/>
+      <c r="AR37" s="3"/>
+      <c r="AS37" s="3"/>
+      <c r="AT37" s="3"/>
+      <c r="AU37" s="3"/>
+      <c r="AV37" s="3"/>
+      <c r="AW37" s="3"/>
+      <c r="AX37" s="3"/>
+      <c r="AY37" s="3"/>
+      <c r="AZ37" s="3"/>
+      <c r="BA37" s="3"/>
+      <c r="BB37" s="3"/>
+      <c r="BC37" s="3"/>
+      <c r="BD37" s="3"/>
+      <c r="BE37" s="3"/>
+      <c r="BF37" s="3"/>
+      <c r="BG37" s="3"/>
+      <c r="BH37" s="3"/>
+      <c r="BI37" s="3"/>
+      <c r="BJ37" s="3"/>
     </row>
     <row r="38" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -6764,35 +6764,35 @@
       <c r="AF38">
         <v>0</v>
       </c>
-      <c r="AH38" s="4"/>
-      <c r="AI38" s="4"/>
-      <c r="AJ38" s="4"/>
-      <c r="AK38" s="4"/>
-      <c r="AL38" s="4"/>
-      <c r="AM38" s="4"/>
-      <c r="AN38" s="4"/>
-      <c r="AO38" s="4"/>
-      <c r="AP38" s="4"/>
-      <c r="AQ38" s="4"/>
-      <c r="AR38" s="4"/>
-      <c r="AS38" s="4"/>
-      <c r="AT38" s="4"/>
-      <c r="AU38" s="4"/>
-      <c r="AV38" s="4"/>
-      <c r="AW38" s="4"/>
-      <c r="AX38" s="4"/>
-      <c r="AY38" s="4"/>
-      <c r="AZ38" s="4"/>
-      <c r="BA38" s="4"/>
-      <c r="BB38" s="4"/>
-      <c r="BC38" s="4"/>
-      <c r="BD38" s="4"/>
-      <c r="BE38" s="4"/>
-      <c r="BF38" s="4"/>
-      <c r="BG38" s="4"/>
-      <c r="BH38" s="4"/>
-      <c r="BI38" s="4"/>
-      <c r="BJ38" s="4"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="3"/>
+      <c r="AJ38" s="3"/>
+      <c r="AK38" s="3"/>
+      <c r="AL38" s="3"/>
+      <c r="AM38" s="3"/>
+      <c r="AN38" s="3"/>
+      <c r="AO38" s="3"/>
+      <c r="AP38" s="3"/>
+      <c r="AQ38" s="3"/>
+      <c r="AR38" s="3"/>
+      <c r="AS38" s="3"/>
+      <c r="AT38" s="3"/>
+      <c r="AU38" s="3"/>
+      <c r="AV38" s="3"/>
+      <c r="AW38" s="3"/>
+      <c r="AX38" s="3"/>
+      <c r="AY38" s="3"/>
+      <c r="AZ38" s="3"/>
+      <c r="BA38" s="3"/>
+      <c r="BB38" s="3"/>
+      <c r="BC38" s="3"/>
+      <c r="BD38" s="3"/>
+      <c r="BE38" s="3"/>
+      <c r="BF38" s="3"/>
+      <c r="BG38" s="3"/>
+      <c r="BH38" s="3"/>
+      <c r="BI38" s="3"/>
+      <c r="BJ38" s="3"/>
     </row>
     <row r="39" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -6891,35 +6891,35 @@
       <c r="AF39">
         <v>0</v>
       </c>
-      <c r="AH39" s="4"/>
-      <c r="AI39" s="4"/>
-      <c r="AJ39" s="4"/>
-      <c r="AK39" s="4"/>
-      <c r="AL39" s="4"/>
-      <c r="AM39" s="4"/>
-      <c r="AN39" s="4"/>
-      <c r="AO39" s="4"/>
-      <c r="AP39" s="4"/>
-      <c r="AQ39" s="4"/>
-      <c r="AR39" s="4"/>
-      <c r="AS39" s="4"/>
-      <c r="AT39" s="4"/>
-      <c r="AU39" s="4"/>
-      <c r="AV39" s="4"/>
-      <c r="AW39" s="4"/>
-      <c r="AX39" s="4"/>
-      <c r="AY39" s="4"/>
-      <c r="AZ39" s="4"/>
-      <c r="BA39" s="4"/>
-      <c r="BB39" s="4"/>
-      <c r="BC39" s="4"/>
-      <c r="BD39" s="4"/>
-      <c r="BE39" s="4"/>
-      <c r="BF39" s="4"/>
-      <c r="BG39" s="4"/>
-      <c r="BH39" s="4"/>
-      <c r="BI39" s="4"/>
-      <c r="BJ39" s="4"/>
+      <c r="AH39" s="3"/>
+      <c r="AI39" s="3"/>
+      <c r="AJ39" s="3"/>
+      <c r="AK39" s="3"/>
+      <c r="AL39" s="3"/>
+      <c r="AM39" s="3"/>
+      <c r="AN39" s="3"/>
+      <c r="AO39" s="3"/>
+      <c r="AP39" s="3"/>
+      <c r="AQ39" s="3"/>
+      <c r="AR39" s="3"/>
+      <c r="AS39" s="3"/>
+      <c r="AT39" s="3"/>
+      <c r="AU39" s="3"/>
+      <c r="AV39" s="3"/>
+      <c r="AW39" s="3"/>
+      <c r="AX39" s="3"/>
+      <c r="AY39" s="3"/>
+      <c r="AZ39" s="3"/>
+      <c r="BA39" s="3"/>
+      <c r="BB39" s="3"/>
+      <c r="BC39" s="3"/>
+      <c r="BD39" s="3"/>
+      <c r="BE39" s="3"/>
+      <c r="BF39" s="3"/>
+      <c r="BG39" s="3"/>
+      <c r="BH39" s="3"/>
+      <c r="BI39" s="3"/>
+      <c r="BJ39" s="3"/>
     </row>
     <row r="40" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -7018,35 +7018,35 @@
       <c r="AF40">
         <v>0</v>
       </c>
-      <c r="AH40" s="4"/>
-      <c r="AI40" s="4"/>
-      <c r="AJ40" s="4"/>
-      <c r="AK40" s="4"/>
-      <c r="AL40" s="4"/>
-      <c r="AM40" s="4"/>
-      <c r="AN40" s="4"/>
-      <c r="AO40" s="4"/>
-      <c r="AP40" s="4"/>
-      <c r="AQ40" s="4"/>
-      <c r="AR40" s="4"/>
-      <c r="AS40" s="4"/>
-      <c r="AT40" s="4"/>
-      <c r="AU40" s="4"/>
-      <c r="AV40" s="4"/>
-      <c r="AW40" s="4"/>
-      <c r="AX40" s="4"/>
-      <c r="AY40" s="4"/>
-      <c r="AZ40" s="4"/>
-      <c r="BA40" s="4"/>
-      <c r="BB40" s="4"/>
-      <c r="BC40" s="4"/>
-      <c r="BD40" s="4"/>
-      <c r="BE40" s="4"/>
-      <c r="BF40" s="4"/>
-      <c r="BG40" s="4"/>
-      <c r="BH40" s="4"/>
-      <c r="BI40" s="4"/>
-      <c r="BJ40" s="4"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="3"/>
+      <c r="AK40" s="3"/>
+      <c r="AL40" s="3"/>
+      <c r="AM40" s="3"/>
+      <c r="AN40" s="3"/>
+      <c r="AO40" s="3"/>
+      <c r="AP40" s="3"/>
+      <c r="AQ40" s="3"/>
+      <c r="AR40" s="3"/>
+      <c r="AS40" s="3"/>
+      <c r="AT40" s="3"/>
+      <c r="AU40" s="3"/>
+      <c r="AV40" s="3"/>
+      <c r="AW40" s="3"/>
+      <c r="AX40" s="3"/>
+      <c r="AY40" s="3"/>
+      <c r="AZ40" s="3"/>
+      <c r="BA40" s="3"/>
+      <c r="BB40" s="3"/>
+      <c r="BC40" s="3"/>
+      <c r="BD40" s="3"/>
+      <c r="BE40" s="3"/>
+      <c r="BF40" s="3"/>
+      <c r="BG40" s="3"/>
+      <c r="BH40" s="3"/>
+      <c r="BI40" s="3"/>
+      <c r="BJ40" s="3"/>
     </row>
     <row r="41" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -7145,35 +7145,35 @@
       <c r="AF41">
         <v>0</v>
       </c>
-      <c r="AH41" s="4"/>
-      <c r="AI41" s="4"/>
-      <c r="AJ41" s="4"/>
-      <c r="AK41" s="4"/>
-      <c r="AL41" s="4"/>
-      <c r="AM41" s="4"/>
-      <c r="AN41" s="4"/>
-      <c r="AO41" s="4"/>
-      <c r="AP41" s="4"/>
-      <c r="AQ41" s="4"/>
-      <c r="AR41" s="4"/>
-      <c r="AS41" s="4"/>
-      <c r="AT41" s="4"/>
-      <c r="AU41" s="4"/>
-      <c r="AV41" s="4"/>
-      <c r="AW41" s="4"/>
-      <c r="AX41" s="4"/>
-      <c r="AY41" s="4"/>
-      <c r="AZ41" s="4"/>
-      <c r="BA41" s="4"/>
-      <c r="BB41" s="4"/>
-      <c r="BC41" s="4"/>
-      <c r="BD41" s="4"/>
-      <c r="BE41" s="4"/>
-      <c r="BF41" s="4"/>
-      <c r="BG41" s="4"/>
-      <c r="BH41" s="4"/>
-      <c r="BI41" s="4"/>
-      <c r="BJ41" s="4"/>
+      <c r="AH41" s="3"/>
+      <c r="AI41" s="3"/>
+      <c r="AJ41" s="3"/>
+      <c r="AK41" s="3"/>
+      <c r="AL41" s="3"/>
+      <c r="AM41" s="3"/>
+      <c r="AN41" s="3"/>
+      <c r="AO41" s="3"/>
+      <c r="AP41" s="3"/>
+      <c r="AQ41" s="3"/>
+      <c r="AR41" s="3"/>
+      <c r="AS41" s="3"/>
+      <c r="AT41" s="3"/>
+      <c r="AU41" s="3"/>
+      <c r="AV41" s="3"/>
+      <c r="AW41" s="3"/>
+      <c r="AX41" s="3"/>
+      <c r="AY41" s="3"/>
+      <c r="AZ41" s="3"/>
+      <c r="BA41" s="3"/>
+      <c r="BB41" s="3"/>
+      <c r="BC41" s="3"/>
+      <c r="BD41" s="3"/>
+      <c r="BE41" s="3"/>
+      <c r="BF41" s="3"/>
+      <c r="BG41" s="3"/>
+      <c r="BH41" s="3"/>
+      <c r="BI41" s="3"/>
+      <c r="BJ41" s="3"/>
     </row>
     <row r="42" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -7272,35 +7272,35 @@
       <c r="AF42">
         <v>0</v>
       </c>
-      <c r="AH42" s="4"/>
-      <c r="AI42" s="4"/>
-      <c r="AJ42" s="4"/>
-      <c r="AK42" s="4"/>
-      <c r="AL42" s="4"/>
-      <c r="AM42" s="4"/>
-      <c r="AN42" s="4"/>
-      <c r="AO42" s="4"/>
-      <c r="AP42" s="4"/>
-      <c r="AQ42" s="4"/>
-      <c r="AR42" s="4"/>
-      <c r="AS42" s="4"/>
-      <c r="AT42" s="4"/>
-      <c r="AU42" s="4"/>
-      <c r="AV42" s="4"/>
-      <c r="AW42" s="4"/>
-      <c r="AX42" s="4"/>
-      <c r="AY42" s="4"/>
-      <c r="AZ42" s="4"/>
-      <c r="BA42" s="4"/>
-      <c r="BB42" s="4"/>
-      <c r="BC42" s="4"/>
-      <c r="BD42" s="4"/>
-      <c r="BE42" s="4"/>
-      <c r="BF42" s="4"/>
-      <c r="BG42" s="4"/>
-      <c r="BH42" s="4"/>
-      <c r="BI42" s="4"/>
-      <c r="BJ42" s="4"/>
+      <c r="AH42" s="3"/>
+      <c r="AI42" s="3"/>
+      <c r="AJ42" s="3"/>
+      <c r="AK42" s="3"/>
+      <c r="AL42" s="3"/>
+      <c r="AM42" s="3"/>
+      <c r="AN42" s="3"/>
+      <c r="AO42" s="3"/>
+      <c r="AP42" s="3"/>
+      <c r="AQ42" s="3"/>
+      <c r="AR42" s="3"/>
+      <c r="AS42" s="3"/>
+      <c r="AT42" s="3"/>
+      <c r="AU42" s="3"/>
+      <c r="AV42" s="3"/>
+      <c r="AW42" s="3"/>
+      <c r="AX42" s="3"/>
+      <c r="AY42" s="3"/>
+      <c r="AZ42" s="3"/>
+      <c r="BA42" s="3"/>
+      <c r="BB42" s="3"/>
+      <c r="BC42" s="3"/>
+      <c r="BD42" s="3"/>
+      <c r="BE42" s="3"/>
+      <c r="BF42" s="3"/>
+      <c r="BG42" s="3"/>
+      <c r="BH42" s="3"/>
+      <c r="BI42" s="3"/>
+      <c r="BJ42" s="3"/>
     </row>
     <row r="43" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -7399,35 +7399,35 @@
       <c r="AF43">
         <v>0</v>
       </c>
-      <c r="AH43" s="4"/>
-      <c r="AI43" s="4"/>
-      <c r="AJ43" s="4"/>
-      <c r="AK43" s="4"/>
-      <c r="AL43" s="4"/>
-      <c r="AM43" s="4"/>
-      <c r="AN43" s="4"/>
-      <c r="AO43" s="4"/>
-      <c r="AP43" s="4"/>
-      <c r="AQ43" s="4"/>
-      <c r="AR43" s="4"/>
-      <c r="AS43" s="4"/>
-      <c r="AT43" s="4"/>
-      <c r="AU43" s="4"/>
-      <c r="AV43" s="4"/>
-      <c r="AW43" s="4"/>
-      <c r="AX43" s="4"/>
-      <c r="AY43" s="4"/>
-      <c r="AZ43" s="4"/>
-      <c r="BA43" s="4"/>
-      <c r="BB43" s="4"/>
-      <c r="BC43" s="4"/>
-      <c r="BD43" s="4"/>
-      <c r="BE43" s="4"/>
-      <c r="BF43" s="4"/>
-      <c r="BG43" s="4"/>
-      <c r="BH43" s="4"/>
-      <c r="BI43" s="4"/>
-      <c r="BJ43" s="4"/>
+      <c r="AH43" s="3"/>
+      <c r="AI43" s="3"/>
+      <c r="AJ43" s="3"/>
+      <c r="AK43" s="3"/>
+      <c r="AL43" s="3"/>
+      <c r="AM43" s="3"/>
+      <c r="AN43" s="3"/>
+      <c r="AO43" s="3"/>
+      <c r="AP43" s="3"/>
+      <c r="AQ43" s="3"/>
+      <c r="AR43" s="3"/>
+      <c r="AS43" s="3"/>
+      <c r="AT43" s="3"/>
+      <c r="AU43" s="3"/>
+      <c r="AV43" s="3"/>
+      <c r="AW43" s="3"/>
+      <c r="AX43" s="3"/>
+      <c r="AY43" s="3"/>
+      <c r="AZ43" s="3"/>
+      <c r="BA43" s="3"/>
+      <c r="BB43" s="3"/>
+      <c r="BC43" s="3"/>
+      <c r="BD43" s="3"/>
+      <c r="BE43" s="3"/>
+      <c r="BF43" s="3"/>
+      <c r="BG43" s="3"/>
+      <c r="BH43" s="3"/>
+      <c r="BI43" s="3"/>
+      <c r="BJ43" s="3"/>
     </row>
     <row r="44" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -7526,35 +7526,35 @@
       <c r="AF44">
         <v>0</v>
       </c>
-      <c r="AH44" s="4"/>
-      <c r="AI44" s="4"/>
-      <c r="AJ44" s="4"/>
-      <c r="AK44" s="4"/>
-      <c r="AL44" s="4"/>
-      <c r="AM44" s="4"/>
-      <c r="AN44" s="4"/>
-      <c r="AO44" s="4"/>
-      <c r="AP44" s="4"/>
-      <c r="AQ44" s="4"/>
-      <c r="AR44" s="4"/>
-      <c r="AS44" s="4"/>
-      <c r="AT44" s="4"/>
-      <c r="AU44" s="4"/>
-      <c r="AV44" s="4"/>
-      <c r="AW44" s="4"/>
-      <c r="AX44" s="4"/>
-      <c r="AY44" s="4"/>
-      <c r="AZ44" s="4"/>
-      <c r="BA44" s="4"/>
-      <c r="BB44" s="4"/>
-      <c r="BC44" s="4"/>
-      <c r="BD44" s="4"/>
-      <c r="BE44" s="4"/>
-      <c r="BF44" s="4"/>
-      <c r="BG44" s="4"/>
-      <c r="BH44" s="4"/>
-      <c r="BI44" s="4"/>
-      <c r="BJ44" s="4"/>
+      <c r="AH44" s="3"/>
+      <c r="AI44" s="3"/>
+      <c r="AJ44" s="3"/>
+      <c r="AK44" s="3"/>
+      <c r="AL44" s="3"/>
+      <c r="AM44" s="3"/>
+      <c r="AN44" s="3"/>
+      <c r="AO44" s="3"/>
+      <c r="AP44" s="3"/>
+      <c r="AQ44" s="3"/>
+      <c r="AR44" s="3"/>
+      <c r="AS44" s="3"/>
+      <c r="AT44" s="3"/>
+      <c r="AU44" s="3"/>
+      <c r="AV44" s="3"/>
+      <c r="AW44" s="3"/>
+      <c r="AX44" s="3"/>
+      <c r="AY44" s="3"/>
+      <c r="AZ44" s="3"/>
+      <c r="BA44" s="3"/>
+      <c r="BB44" s="3"/>
+      <c r="BC44" s="3"/>
+      <c r="BD44" s="3"/>
+      <c r="BE44" s="3"/>
+      <c r="BF44" s="3"/>
+      <c r="BG44" s="3"/>
+      <c r="BH44" s="3"/>
+      <c r="BI44" s="3"/>
+      <c r="BJ44" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7572,23 +7572,23 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
@@ -12017,13 +12017,13 @@
   <dimension ref="A1:AF45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>381</v>
       </c>
       <c r="R1" s="1"/>

</xml_diff>

<commit_message>
Removed arenicola from figures and separated tables
</commit_message>
<xml_diff>
--- a/data/allMetaboliteData.xlsx
+++ b/data/allMetaboliteData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E67E0A-1D40-4D7B-99EC-9DF1526EF06F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476B7C32-671F-4C78-A6BC-1A4FF2B28DA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13530" yWindow="6675" windowWidth="15375" windowHeight="8370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fresh" sheetId="1" r:id="rId1"/>
@@ -2085,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ44"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12016,7 +12016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1B6054-9053-4986-AAC3-C5A8F449423C}">
   <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>

</xml_diff>